<commit_message>
Deploying to gh-pages from  @ 624c151c0cd88840eabfaeb857fa1caa3aeb4b92 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2025_5-1-1.xlsx
+++ b/assets/excel/2025_5-1-1.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15_Uebergreifende_Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC743AE4-99E8-4B71-B459-1DBA2BF6AFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8902C74F-2911-4D60-8D13-28D90C39C994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{FAA839E9-FEB0-4C88-9D08-E3A9182EBE0D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{FAA839E9-FEB0-4C88-9D08-E3A9182EBE0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -458,30 +461,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -489,21 +468,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -546,20 +510,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -588,6 +540,57 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -909,7 +912,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:I175"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -935,2758 +938,2758 @@
       <c r="C4" s="3"/>
     </row>
     <row r="6" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
     </row>
     <row r="7" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
     </row>
     <row r="8" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="12" t="s">
+      <c r="B8" s="35"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17">
+      <c r="B9" s="36"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="44">
         <v>1000</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="19"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="46"/>
     </row>
     <row r="10" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="27">
         <v>2024</v>
       </c>
-      <c r="D11" s="45">
+      <c r="D11" s="28">
         <v>7.6138599999999999</v>
       </c>
-      <c r="E11" s="45">
+      <c r="E11" s="28">
         <v>4.5187400000000002</v>
       </c>
-      <c r="F11" s="45">
+      <c r="F11" s="28">
         <v>12.1326</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="44">
+      <c r="C12" s="27">
         <v>2024</v>
       </c>
-      <c r="D12" s="45">
+      <c r="D12" s="28">
         <v>143.77341000000001</v>
       </c>
-      <c r="E12" s="45">
+      <c r="E12" s="28">
         <v>47.101289999999999</v>
       </c>
-      <c r="F12" s="45">
+      <c r="F12" s="28">
         <v>190.87470000000002</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="27">
         <v>2024</v>
       </c>
-      <c r="D13" s="45">
+      <c r="D13" s="28">
         <v>10.22898</v>
       </c>
-      <c r="E13" s="45">
+      <c r="E13" s="28">
         <v>2.0726199999999997</v>
       </c>
-      <c r="F13" s="45">
+      <c r="F13" s="28">
         <v>12.301600000000001</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="44">
+      <c r="C14" s="27">
         <v>2024</v>
       </c>
-      <c r="D14" s="45">
+      <c r="D14" s="28">
         <v>64.89461</v>
       </c>
-      <c r="E14" s="45">
+      <c r="E14" s="28">
         <v>6.4905799999999996</v>
       </c>
-      <c r="F14" s="45">
+      <c r="F14" s="28">
         <v>71.385190000000009</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="44">
+      <c r="C15" s="27">
         <v>2024</v>
       </c>
-      <c r="D15" s="45">
+      <c r="D15" s="28">
         <v>74.241479999999996</v>
       </c>
-      <c r="E15" s="45">
+      <c r="E15" s="28">
         <v>63.077260000000003</v>
       </c>
-      <c r="F15" s="45">
+      <c r="F15" s="28">
         <v>137.31873999999999</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="27">
         <v>2024</v>
       </c>
-      <c r="D16" s="45">
+      <c r="D16" s="28">
         <v>71.272009999999995</v>
       </c>
-      <c r="E16" s="45">
+      <c r="E16" s="28">
         <v>17.785029999999999</v>
       </c>
-      <c r="F16" s="45">
+      <c r="F16" s="28">
         <v>89.057040000000001</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="27">
         <v>2024</v>
       </c>
-      <c r="D17" s="45">
+      <c r="D17" s="28">
         <v>34.177410000000002</v>
       </c>
-      <c r="E17" s="45">
+      <c r="E17" s="28">
         <v>28.967449999999999</v>
       </c>
-      <c r="F17" s="45">
+      <c r="F17" s="28">
         <v>63.144849999999998</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="44">
+      <c r="C18" s="27">
         <v>2024</v>
       </c>
-      <c r="D18" s="45">
+      <c r="D18" s="28">
         <v>61.485489999999999</v>
       </c>
-      <c r="E18" s="45">
+      <c r="E18" s="28">
         <v>65.580380000000005</v>
       </c>
-      <c r="F18" s="45">
+      <c r="F18" s="28">
         <v>127.06586999999999</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="44">
+      <c r="C19" s="27">
         <v>2024</v>
       </c>
-      <c r="D19" s="45">
+      <c r="D19" s="28">
         <v>54.651580000000003</v>
       </c>
-      <c r="E19" s="45">
+      <c r="E19" s="28">
         <v>166.15282999999999</v>
       </c>
-      <c r="F19" s="45">
+      <c r="F19" s="28">
         <v>220.80440999999999</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="44">
+      <c r="C20" s="27">
         <v>2024</v>
       </c>
-      <c r="D20" s="45">
+      <c r="D20" s="28">
         <v>18.612500000000001</v>
       </c>
-      <c r="E20" s="45">
+      <c r="E20" s="28">
         <v>23.612830000000002</v>
       </c>
-      <c r="F20" s="45">
+      <c r="F20" s="28">
         <v>42.22533</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="44">
+      <c r="C21" s="27">
         <v>2024</v>
       </c>
-      <c r="D21" s="47">
+      <c r="D21" s="30">
         <v>541.58618999999999</v>
       </c>
-      <c r="E21" s="47">
+      <c r="E21" s="30">
         <v>429.34171000000003</v>
       </c>
-      <c r="F21" s="47">
+      <c r="F21" s="30">
         <v>970.92789000000005</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="44">
+      <c r="C22" s="27">
         <v>2023</v>
       </c>
-      <c r="D22" s="45">
+      <c r="D22" s="28">
         <v>7.2283599999999995</v>
       </c>
-      <c r="E22" s="45">
+      <c r="E22" s="28">
         <v>4.0915300000000006</v>
       </c>
-      <c r="F22" s="45">
+      <c r="F22" s="28">
         <v>11.319889999999999</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="44">
+      <c r="C23" s="27">
         <v>2023</v>
       </c>
-      <c r="D23" s="45">
+      <c r="D23" s="28">
         <v>145.58401999999998</v>
       </c>
-      <c r="E23" s="45">
+      <c r="E23" s="28">
         <v>43.074120000000001</v>
       </c>
-      <c r="F23" s="45">
+      <c r="F23" s="28">
         <v>188.65814</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="44">
+      <c r="C24" s="27">
         <v>2023</v>
       </c>
-      <c r="D24" s="45">
+      <c r="D24" s="28">
         <v>7.2332799999999997</v>
       </c>
-      <c r="E24" s="45">
+      <c r="E24" s="28">
         <v>2.3273800000000002</v>
       </c>
-      <c r="F24" s="45">
+      <c r="F24" s="28">
         <v>9.5606600000000004</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="44">
+      <c r="C25" s="27">
         <v>2023</v>
       </c>
-      <c r="D25" s="45">
+      <c r="D25" s="28">
         <v>64.071619999999996</v>
       </c>
-      <c r="E25" s="45">
+      <c r="E25" s="28">
         <v>6.5575799999999997</v>
       </c>
-      <c r="F25" s="45">
+      <c r="F25" s="28">
         <v>70.629199999999997</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="44">
+      <c r="C26" s="27">
         <v>2023</v>
       </c>
-      <c r="D26" s="45">
+      <c r="D26" s="28">
         <v>68.132649999999998</v>
       </c>
-      <c r="E26" s="45">
+      <c r="E26" s="28">
         <v>62.94426</v>
       </c>
-      <c r="F26" s="45">
+      <c r="F26" s="28">
         <v>131.07691</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="44">
+      <c r="C27" s="27">
         <v>2023</v>
       </c>
-      <c r="D27" s="45">
+      <c r="D27" s="28">
         <v>67.140710000000013</v>
       </c>
-      <c r="E27" s="45">
+      <c r="E27" s="28">
         <v>21.851749999999999</v>
       </c>
-      <c r="F27" s="45">
+      <c r="F27" s="28">
         <v>88.992460000000008</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="44">
+      <c r="C28" s="27">
         <v>2023</v>
       </c>
-      <c r="D28" s="45">
+      <c r="D28" s="28">
         <v>34.844080000000005</v>
       </c>
-      <c r="E28" s="45">
+      <c r="E28" s="28">
         <v>26.783619999999999</v>
       </c>
-      <c r="F28" s="45">
+      <c r="F28" s="28">
         <v>61.627699999999997</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="44">
+      <c r="C29" s="27">
         <v>2023</v>
       </c>
-      <c r="D29" s="45">
+      <c r="D29" s="28">
         <v>55.297220000000003</v>
       </c>
-      <c r="E29" s="45">
+      <c r="E29" s="28">
         <v>59.164199999999994</v>
       </c>
-      <c r="F29" s="45">
+      <c r="F29" s="28">
         <v>114.46142</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="43" t="s">
+      <c r="B30" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="44">
+      <c r="C30" s="27">
         <v>2023</v>
       </c>
-      <c r="D30" s="45">
+      <c r="D30" s="28">
         <v>53.854199999999999</v>
       </c>
-      <c r="E30" s="45">
+      <c r="E30" s="28">
         <v>149.73727</v>
       </c>
-      <c r="F30" s="45">
+      <c r="F30" s="28">
         <v>203.59147000000002</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="44">
+      <c r="C31" s="27">
         <v>2023</v>
       </c>
-      <c r="D31" s="45">
+      <c r="D31" s="28">
         <v>16.445919999999997</v>
       </c>
-      <c r="E31" s="45">
+      <c r="E31" s="28">
         <v>23.032299999999999</v>
       </c>
-      <c r="F31" s="45">
+      <c r="F31" s="28">
         <v>39.478209999999997</v>
       </c>
-      <c r="I31" s="42"/>
-    </row>
-    <row r="32" spans="2:9" s="21" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="46" t="s">
+      <c r="I31" s="25"/>
+    </row>
+    <row r="32" spans="2:9" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="48">
+      <c r="C32" s="31">
         <v>2023</v>
       </c>
-      <c r="D32" s="47">
+      <c r="D32" s="30">
         <v>520.05517999999995</v>
       </c>
-      <c r="E32" s="47">
+      <c r="E32" s="30">
         <v>403.31663000000003</v>
       </c>
-      <c r="F32" s="47">
+      <c r="F32" s="30">
         <v>923.3718100000001</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="44">
+      <c r="C33" s="27">
         <v>2022</v>
       </c>
-      <c r="D33" s="45">
+      <c r="D33" s="28">
         <v>9.1918700000000015</v>
       </c>
-      <c r="E33" s="45">
+      <c r="E33" s="28">
         <v>4.94754</v>
       </c>
-      <c r="F33" s="45">
+      <c r="F33" s="28">
         <v>14.13941</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="23">
+      <c r="C34" s="10">
         <v>2022</v>
       </c>
-      <c r="D34" s="24">
+      <c r="D34" s="11">
         <v>153.34922</v>
       </c>
-      <c r="E34" s="24">
+      <c r="E34" s="11">
         <v>47.124540000000003</v>
       </c>
-      <c r="F34" s="24">
+      <c r="F34" s="11">
         <v>200.47375</v>
       </c>
     </row>
     <row r="35" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="23">
+      <c r="C35" s="10">
         <v>2022</v>
       </c>
-      <c r="D35" s="24">
+      <c r="D35" s="11">
         <v>6.1797599999999999</v>
       </c>
-      <c r="E35" s="24">
+      <c r="E35" s="11">
         <v>2.2815100000000004</v>
       </c>
-      <c r="F35" s="24">
+      <c r="F35" s="11">
         <v>8.4612700000000007</v>
       </c>
     </row>
     <row r="36" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="23">
+      <c r="C36" s="10">
         <v>2022</v>
       </c>
-      <c r="D36" s="24">
+      <c r="D36" s="11">
         <v>63.33437</v>
       </c>
-      <c r="E36" s="24">
+      <c r="E36" s="11">
         <v>7.6503699999999997</v>
       </c>
-      <c r="F36" s="24">
+      <c r="F36" s="11">
         <v>70.984740000000002</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="23">
+      <c r="C37" s="10">
         <v>2022</v>
       </c>
-      <c r="D37" s="24">
+      <c r="D37" s="11">
         <v>70.136719999999997</v>
       </c>
-      <c r="E37" s="24">
+      <c r="E37" s="11">
         <v>63.268720000000002</v>
       </c>
-      <c r="F37" s="24">
+      <c r="F37" s="11">
         <v>133.40544</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="23">
+      <c r="C38" s="10">
         <v>2022</v>
       </c>
-      <c r="D38" s="24">
+      <c r="D38" s="11">
         <v>68.138149999999996</v>
       </c>
-      <c r="E38" s="24">
+      <c r="E38" s="11">
         <v>18.284689999999998</v>
       </c>
-      <c r="F38" s="24">
+      <c r="F38" s="11">
         <v>86.422839999999994</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="23">
+      <c r="C39" s="10">
         <v>2022</v>
       </c>
-      <c r="D39" s="24">
+      <c r="D39" s="11">
         <v>32.449619999999996</v>
       </c>
-      <c r="E39" s="24">
+      <c r="E39" s="11">
         <v>28.196099999999998</v>
       </c>
-      <c r="F39" s="24">
+      <c r="F39" s="11">
         <v>60.645720000000004</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="23">
+      <c r="C40" s="10">
         <v>2022</v>
       </c>
-      <c r="D40" s="24">
+      <c r="D40" s="11">
         <v>52.007330000000003</v>
       </c>
-      <c r="E40" s="24">
+      <c r="E40" s="11">
         <v>63.224550000000001</v>
       </c>
-      <c r="F40" s="24">
+      <c r="F40" s="11">
         <v>115.23188</v>
       </c>
     </row>
     <row r="41" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="23">
+      <c r="C41" s="10">
         <v>2022</v>
       </c>
-      <c r="D41" s="24">
+      <c r="D41" s="11">
         <v>52.098239999999997</v>
       </c>
-      <c r="E41" s="24">
+      <c r="E41" s="11">
         <v>146.35162</v>
       </c>
-      <c r="F41" s="24">
+      <c r="F41" s="11">
         <v>198.44985999999997</v>
       </c>
     </row>
     <row r="42" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="23">
+      <c r="C42" s="10">
         <v>2022</v>
       </c>
-      <c r="D42" s="24">
+      <c r="D42" s="11">
         <v>21.653080000000003</v>
       </c>
-      <c r="E42" s="24">
+      <c r="E42" s="11">
         <v>25.627209999999998</v>
       </c>
-      <c r="F42" s="24">
+      <c r="F42" s="11">
         <v>47.280279999999998</v>
       </c>
     </row>
-    <row r="43" spans="2:6" s="21" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="25" t="s">
+    <row r="43" spans="2:6" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C43" s="26">
+      <c r="C43" s="13">
         <v>2022</v>
       </c>
-      <c r="D43" s="27">
+      <c r="D43" s="14">
         <v>528.98162000000002</v>
       </c>
-      <c r="E43" s="27">
+      <c r="E43" s="14">
         <v>412.52028999999999</v>
       </c>
-      <c r="F43" s="27">
+      <c r="F43" s="14">
         <v>941.50191000000007</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="23">
+      <c r="C44" s="10">
         <v>2021</v>
       </c>
-      <c r="D44" s="24">
+      <c r="D44" s="11">
         <v>10.572479999999999</v>
       </c>
-      <c r="E44" s="24">
+      <c r="E44" s="11">
         <v>5.7420299999999997</v>
       </c>
-      <c r="F44" s="24">
+      <c r="F44" s="11">
         <v>16.314509999999999</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="23">
+      <c r="C45" s="10">
         <v>2021</v>
       </c>
-      <c r="D45" s="24">
+      <c r="D45" s="11">
         <v>149.85901999999999</v>
       </c>
-      <c r="E45" s="24">
+      <c r="E45" s="11">
         <v>44.907690000000002</v>
       </c>
-      <c r="F45" s="24">
+      <c r="F45" s="11">
         <v>194.76670999999999</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="22" t="s">
+      <c r="B46" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="23">
+      <c r="C46" s="10">
         <v>2021</v>
       </c>
-      <c r="D46" s="24">
+      <c r="D46" s="11">
         <v>6.6376800000000005</v>
       </c>
-      <c r="E46" s="24">
+      <c r="E46" s="11">
         <v>2.4217399999999998</v>
       </c>
-      <c r="F46" s="24">
+      <c r="F46" s="11">
         <v>9.0594099999999997</v>
       </c>
     </row>
     <row r="47" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="22" t="s">
+      <c r="B47" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="23">
+      <c r="C47" s="10">
         <v>2021</v>
       </c>
-      <c r="D47" s="24">
+      <c r="D47" s="11">
         <v>55.948300000000003</v>
       </c>
-      <c r="E47" s="24">
+      <c r="E47" s="11">
         <v>5.4960900000000006</v>
       </c>
-      <c r="F47" s="24">
+      <c r="F47" s="11">
         <v>61.444389999999999</v>
       </c>
     </row>
     <row r="48" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="22" t="s">
+      <c r="B48" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="23">
+      <c r="C48" s="10">
         <v>2021</v>
       </c>
-      <c r="D48" s="24">
+      <c r="D48" s="11">
         <v>64.33099</v>
       </c>
-      <c r="E48" s="24">
+      <c r="E48" s="11">
         <v>57.132109999999997</v>
       </c>
-      <c r="F48" s="24">
+      <c r="F48" s="11">
         <v>121.46310000000001</v>
       </c>
     </row>
     <row r="49" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="22" t="s">
+      <c r="B49" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="23">
+      <c r="C49" s="10">
         <v>2021</v>
       </c>
-      <c r="D49" s="24">
+      <c r="D49" s="11">
         <v>58.601759999999999</v>
       </c>
-      <c r="E49" s="24">
+      <c r="E49" s="11">
         <v>17.339259999999999</v>
       </c>
-      <c r="F49" s="24">
+      <c r="F49" s="11">
         <v>75.941029999999998</v>
       </c>
     </row>
     <row r="50" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="23">
+      <c r="C50" s="10">
         <v>2021</v>
       </c>
-      <c r="D50" s="24">
+      <c r="D50" s="11">
         <v>29.5642</v>
       </c>
-      <c r="E50" s="24">
+      <c r="E50" s="11">
         <v>23.365080000000003</v>
       </c>
-      <c r="F50" s="24">
+      <c r="F50" s="11">
         <v>52.929269999999995</v>
       </c>
     </row>
     <row r="51" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="23">
+      <c r="C51" s="10">
         <v>2021</v>
       </c>
-      <c r="D51" s="24">
+      <c r="D51" s="11">
         <v>51.003819999999997</v>
       </c>
-      <c r="E51" s="24">
+      <c r="E51" s="11">
         <v>57.348769999999995</v>
       </c>
-      <c r="F51" s="24">
+      <c r="F51" s="11">
         <v>108.35258999999999</v>
       </c>
     </row>
     <row r="52" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="22" t="s">
+      <c r="B52" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C52" s="23">
+      <c r="C52" s="10">
         <v>2021</v>
       </c>
-      <c r="D52" s="24">
+      <c r="D52" s="11">
         <v>48.759029999999996</v>
       </c>
-      <c r="E52" s="24">
+      <c r="E52" s="11">
         <v>128.91737000000001</v>
       </c>
-      <c r="F52" s="24">
+      <c r="F52" s="11">
         <v>177.67641</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="22" t="s">
+      <c r="B53" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C53" s="23">
+      <c r="C53" s="10">
         <v>2021</v>
       </c>
-      <c r="D53" s="24">
+      <c r="D53" s="11">
         <v>21.010840000000002</v>
       </c>
-      <c r="E53" s="24">
+      <c r="E53" s="11">
         <v>24.691520000000001</v>
       </c>
-      <c r="F53" s="24">
+      <c r="F53" s="11">
         <v>45.702359999999999</v>
       </c>
     </row>
-    <row r="54" spans="2:6" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="25" t="s">
+    <row r="54" spans="2:6" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C54" s="26">
+      <c r="C54" s="13">
         <v>2021</v>
       </c>
-      <c r="D54" s="27">
+      <c r="D54" s="14">
         <v>497.26251000000002</v>
       </c>
-      <c r="E54" s="27">
-        <v>497.26251000000002</v>
-      </c>
-      <c r="F54" s="27">
+      <c r="E54" s="14">
+        <v>375.02</v>
+      </c>
+      <c r="F54" s="14">
         <v>872.29062999999996</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="22" t="s">
+      <c r="B55" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="23">
+      <c r="C55" s="10">
         <v>2019</v>
       </c>
-      <c r="D55" s="24">
+      <c r="D55" s="11">
         <v>8.0970600000000008</v>
       </c>
-      <c r="E55" s="24">
+      <c r="E55" s="11">
         <v>3.3266199999999997</v>
       </c>
-      <c r="F55" s="24">
+      <c r="F55" s="11">
         <v>11.423680000000001</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="22" t="s">
+      <c r="B56" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C56" s="23">
+      <c r="C56" s="10">
         <v>2019</v>
       </c>
-      <c r="D56" s="24">
+      <c r="D56" s="11">
         <v>137.23995000000002</v>
       </c>
-      <c r="E56" s="24">
+      <c r="E56" s="11">
         <v>43.812690000000003</v>
       </c>
-      <c r="F56" s="24">
+      <c r="F56" s="11">
         <v>181.05264000000003</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="23">
+      <c r="C57" s="10">
         <v>2019</v>
       </c>
-      <c r="D57" s="24">
+      <c r="D57" s="11">
         <v>5.8705400000000001</v>
       </c>
-      <c r="E57" s="24">
+      <c r="E57" s="11">
         <v>1.97601</v>
       </c>
-      <c r="F57" s="24">
+      <c r="F57" s="11">
         <v>7.8465500000000006</v>
       </c>
     </row>
     <row r="58" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C58" s="23">
+      <c r="C58" s="10">
         <v>2019</v>
       </c>
-      <c r="D58" s="24">
+      <c r="D58" s="11">
         <v>61.42324</v>
       </c>
-      <c r="E58" s="24">
+      <c r="E58" s="11">
         <v>7.3893900000000006</v>
       </c>
-      <c r="F58" s="24">
+      <c r="F58" s="11">
         <v>68.812629999999999</v>
       </c>
     </row>
     <row r="59" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="22" t="s">
+      <c r="B59" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C59" s="23">
+      <c r="C59" s="10">
         <v>2019</v>
       </c>
-      <c r="D59" s="24">
+      <c r="D59" s="11">
         <v>70.294119999999992</v>
       </c>
-      <c r="E59" s="24">
+      <c r="E59" s="11">
         <v>60.605710000000002</v>
       </c>
-      <c r="F59" s="24">
+      <c r="F59" s="11">
         <v>130.89983000000001</v>
       </c>
     </row>
     <row r="60" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="22" t="s">
+      <c r="B60" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C60" s="23">
+      <c r="C60" s="10">
         <v>2019</v>
       </c>
-      <c r="D60" s="24">
+      <c r="D60" s="11">
         <v>54.424980000000005</v>
       </c>
-      <c r="E60" s="24">
+      <c r="E60" s="11">
         <v>12.738959999999999</v>
       </c>
-      <c r="F60" s="24">
+      <c r="F60" s="11">
         <v>67.163939999999997</v>
       </c>
     </row>
     <row r="61" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="22" t="s">
+      <c r="B61" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C61" s="23">
+      <c r="C61" s="10">
         <v>2019</v>
       </c>
-      <c r="D61" s="24">
+      <c r="D61" s="11">
         <v>31.728919999999999</v>
       </c>
-      <c r="E61" s="24">
+      <c r="E61" s="11">
         <v>25.85134</v>
       </c>
-      <c r="F61" s="24">
+      <c r="F61" s="11">
         <v>57.580260000000003</v>
       </c>
     </row>
     <row r="62" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="23">
+      <c r="C62" s="10">
         <v>2019</v>
       </c>
-      <c r="D62" s="24">
+      <c r="D62" s="11">
         <v>43.846599999999995</v>
       </c>
-      <c r="E62" s="24">
+      <c r="E62" s="11">
         <v>48.489089999999997</v>
       </c>
-      <c r="F62" s="24">
+      <c r="F62" s="11">
         <v>92.335679999999996</v>
       </c>
     </row>
     <row r="63" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="22" t="s">
+      <c r="B63" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C63" s="23">
+      <c r="C63" s="10">
         <v>2019</v>
       </c>
-      <c r="D63" s="24">
+      <c r="D63" s="11">
         <v>43.389919999999996</v>
       </c>
-      <c r="E63" s="24">
+      <c r="E63" s="11">
         <v>117.28994999999999</v>
       </c>
-      <c r="F63" s="24">
+      <c r="F63" s="11">
         <v>160.67986999999999</v>
       </c>
     </row>
     <row r="64" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="22" t="s">
+      <c r="B64" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C64" s="23">
+      <c r="C64" s="10">
         <v>2019</v>
       </c>
-      <c r="D64" s="24">
+      <c r="D64" s="11">
         <v>13.560750000000001</v>
       </c>
-      <c r="E64" s="24">
+      <c r="E64" s="11">
         <v>19.337029999999999</v>
       </c>
-      <c r="F64" s="24">
+      <c r="F64" s="11">
         <v>32.897779999999997</v>
       </c>
     </row>
-    <row r="65" spans="2:6" s="21" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="25" t="s">
+    <row r="65" spans="2:6" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C65" s="26">
+      <c r="C65" s="13">
         <v>2019</v>
       </c>
-      <c r="D65" s="27">
+      <c r="D65" s="14">
         <v>470.17715999999996</v>
       </c>
-      <c r="E65" s="27">
+      <c r="E65" s="14">
         <v>348.16636</v>
       </c>
-      <c r="F65" s="27">
+      <c r="F65" s="14">
         <v>818.34351000000004</v>
       </c>
     </row>
     <row r="66" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="22" t="s">
+      <c r="B66" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C66" s="23">
+      <c r="C66" s="10">
         <v>2018</v>
       </c>
-      <c r="D66" s="24">
+      <c r="D66" s="11">
         <v>9.2372800000000002</v>
       </c>
-      <c r="E66" s="24">
+      <c r="E66" s="11">
         <v>4.9123299999999999</v>
       </c>
-      <c r="F66" s="24">
+      <c r="F66" s="11">
         <v>14.149610000000001</v>
       </c>
     </row>
     <row r="67" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="22" t="s">
+      <c r="B67" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C67" s="23">
+      <c r="C67" s="10">
         <v>2018</v>
       </c>
-      <c r="D67" s="24">
+      <c r="D67" s="11">
         <v>141.85381000000001</v>
       </c>
-      <c r="E67" s="24">
+      <c r="E67" s="11">
         <v>45.829940000000001</v>
       </c>
-      <c r="F67" s="24">
+      <c r="F67" s="11">
         <v>187.68375</v>
       </c>
     </row>
     <row r="68" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="22" t="s">
+      <c r="B68" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C68" s="23">
+      <c r="C68" s="10">
         <v>2018</v>
       </c>
-      <c r="D68" s="24">
+      <c r="D68" s="11">
         <v>6.9294099999999998</v>
       </c>
-      <c r="E68" s="24">
+      <c r="E68" s="11">
         <v>1.99579</v>
       </c>
-      <c r="F68" s="24">
+      <c r="F68" s="11">
         <v>8.9252000000000002</v>
       </c>
     </row>
     <row r="69" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="22" t="s">
+      <c r="B69" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C69" s="23">
+      <c r="C69" s="10">
         <v>2018</v>
       </c>
-      <c r="D69" s="24">
+      <c r="D69" s="11">
         <v>58.642859999999999</v>
       </c>
-      <c r="E69" s="24">
+      <c r="E69" s="11">
         <v>6.5473500000000007</v>
       </c>
-      <c r="F69" s="24">
+      <c r="F69" s="11">
         <v>65.190219999999997</v>
       </c>
     </row>
     <row r="70" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="22" t="s">
+      <c r="B70" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C70" s="23">
+      <c r="C70" s="10">
         <v>2018</v>
       </c>
-      <c r="D70" s="24">
+      <c r="D70" s="11">
         <v>67.828630000000004</v>
       </c>
-      <c r="E70" s="24">
+      <c r="E70" s="11">
         <v>62.089589999999994</v>
       </c>
-      <c r="F70" s="24">
+      <c r="F70" s="11">
         <v>129.91821999999999</v>
       </c>
     </row>
     <row r="71" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="22" t="s">
+      <c r="B71" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C71" s="23">
+      <c r="C71" s="10">
         <v>2018</v>
       </c>
-      <c r="D71" s="24">
+      <c r="D71" s="11">
         <v>50.172239999999995</v>
       </c>
-      <c r="E71" s="24">
+      <c r="E71" s="11">
         <v>11.51253</v>
       </c>
-      <c r="F71" s="24">
+      <c r="F71" s="11">
         <v>61.68477</v>
       </c>
     </row>
     <row r="72" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="22" t="s">
+      <c r="B72" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C72" s="23">
+      <c r="C72" s="10">
         <v>2018</v>
       </c>
-      <c r="D72" s="24">
+      <c r="D72" s="11">
         <v>31.441650000000003</v>
       </c>
-      <c r="E72" s="24">
+      <c r="E72" s="11">
         <v>26.750160000000001</v>
       </c>
-      <c r="F72" s="24">
+      <c r="F72" s="11">
         <v>58.191809999999997</v>
       </c>
     </row>
     <row r="73" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="22" t="s">
+      <c r="B73" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C73" s="23">
+      <c r="C73" s="10">
         <v>2018</v>
       </c>
-      <c r="D73" s="24">
+      <c r="D73" s="11">
         <v>40.487259999999999</v>
       </c>
-      <c r="E73" s="24">
+      <c r="E73" s="11">
         <v>46.75056</v>
       </c>
-      <c r="F73" s="24">
+      <c r="F73" s="11">
         <v>87.237809999999996</v>
       </c>
     </row>
     <row r="74" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="22" t="s">
+      <c r="B74" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C74" s="23">
+      <c r="C74" s="10">
         <v>2018</v>
       </c>
-      <c r="D74" s="24">
+      <c r="D74" s="11">
         <v>42.329569999999997</v>
       </c>
-      <c r="E74" s="24">
+      <c r="E74" s="11">
         <v>113.60674</v>
       </c>
-      <c r="F74" s="24">
+      <c r="F74" s="11">
         <v>155.93630999999999</v>
       </c>
     </row>
     <row r="75" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="22" t="s">
+      <c r="B75" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C75" s="23">
+      <c r="C75" s="10">
         <v>2018</v>
       </c>
-      <c r="D75" s="24">
+      <c r="D75" s="11">
         <v>11.60702</v>
       </c>
-      <c r="E75" s="24">
+      <c r="E75" s="11">
         <v>19.546150000000001</v>
       </c>
-      <c r="F75" s="24">
+      <c r="F75" s="11">
         <v>31.153169999999999</v>
       </c>
     </row>
-    <row r="76" spans="2:6" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="25" t="s">
+    <row r="76" spans="2:6" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C76" s="26">
+      <c r="C76" s="13">
         <v>2018</v>
       </c>
-      <c r="D76" s="27">
+      <c r="D76" s="14">
         <v>460.73616999999996</v>
       </c>
-      <c r="E76" s="27">
+      <c r="E76" s="14">
         <v>345.17609999999996</v>
       </c>
-      <c r="F76" s="27">
+      <c r="F76" s="14">
         <v>805.91227000000003</v>
       </c>
     </row>
     <row r="77" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="22" t="s">
+      <c r="B77" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C77" s="29">
+      <c r="C77" s="16">
         <v>2017</v>
       </c>
-      <c r="D77" s="24">
+      <c r="D77" s="11">
         <v>8.3643600000000013</v>
       </c>
-      <c r="E77" s="24">
+      <c r="E77" s="11">
         <v>3.0600700000000001</v>
       </c>
-      <c r="F77" s="24">
+      <c r="F77" s="11">
         <v>11.424430000000001</v>
       </c>
     </row>
     <row r="78" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="22" t="s">
+      <c r="B78" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C78" s="29">
+      <c r="C78" s="16">
         <v>2017</v>
       </c>
-      <c r="D78" s="24">
+      <c r="D78" s="11">
         <v>143.43660999999997</v>
       </c>
-      <c r="E78" s="24">
+      <c r="E78" s="11">
         <v>41.608449999999998</v>
       </c>
-      <c r="F78" s="24">
+      <c r="F78" s="11">
         <v>185.04506000000001</v>
       </c>
     </row>
     <row r="79" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="22" t="s">
+      <c r="B79" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C79" s="29">
+      <c r="C79" s="16">
         <v>2017</v>
       </c>
-      <c r="D79" s="24">
+      <c r="D79" s="11">
         <v>6.4783299999999997</v>
       </c>
-      <c r="E79" s="24">
+      <c r="E79" s="11">
         <v>1.7835999999999999</v>
       </c>
-      <c r="F79" s="24">
+      <c r="F79" s="11">
         <v>8.2619299999999996</v>
       </c>
     </row>
     <row r="80" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="22" t="s">
+      <c r="B80" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C80" s="29">
+      <c r="C80" s="16">
         <v>2017</v>
       </c>
-      <c r="D80" s="24">
+      <c r="D80" s="11">
         <v>57.102330000000002</v>
       </c>
-      <c r="E80" s="24">
+      <c r="E80" s="11">
         <v>6.4703500000000007</v>
       </c>
-      <c r="F80" s="24">
+      <c r="F80" s="11">
         <v>63.572679999999998</v>
       </c>
     </row>
     <row r="81" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="22" t="s">
+      <c r="B81" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C81" s="29">
+      <c r="C81" s="16">
         <v>2017</v>
       </c>
-      <c r="D81" s="24">
+      <c r="D81" s="11">
         <v>65.751499999999993</v>
       </c>
-      <c r="E81" s="24">
+      <c r="E81" s="11">
         <v>60.129889999999996</v>
       </c>
-      <c r="F81" s="24">
+      <c r="F81" s="11">
         <v>125.8814</v>
       </c>
     </row>
     <row r="82" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="22" t="s">
+      <c r="B82" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C82" s="29">
+      <c r="C82" s="16">
         <v>2017</v>
       </c>
-      <c r="D82" s="24">
+      <c r="D82" s="11">
         <v>48.327449999999999</v>
       </c>
-      <c r="E82" s="24">
+      <c r="E82" s="11">
         <v>12.60933</v>
       </c>
-      <c r="F82" s="24">
+      <c r="F82" s="11">
         <v>60.936779999999999</v>
       </c>
     </row>
     <row r="83" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="22" t="s">
+      <c r="B83" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C83" s="29">
+      <c r="C83" s="16">
         <v>2017</v>
       </c>
-      <c r="D83" s="24">
+      <c r="D83" s="11">
         <v>26.69622</v>
       </c>
-      <c r="E83" s="24">
+      <c r="E83" s="11">
         <v>24.9421</v>
       </c>
-      <c r="F83" s="24">
+      <c r="F83" s="11">
         <v>51.63832</v>
       </c>
     </row>
     <row r="84" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="22" t="s">
+      <c r="B84" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C84" s="29">
+      <c r="C84" s="16">
         <v>2017</v>
       </c>
-      <c r="D84" s="24">
+      <c r="D84" s="11">
         <v>39.163119999999999</v>
       </c>
-      <c r="E84" s="24">
+      <c r="E84" s="11">
         <v>44.583030000000001</v>
       </c>
-      <c r="F84" s="24">
+      <c r="F84" s="11">
         <v>83.74615</v>
       </c>
     </row>
     <row r="85" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="22" t="s">
+      <c r="B85" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C85" s="29">
+      <c r="C85" s="16">
         <v>2017</v>
       </c>
-      <c r="D85" s="24">
+      <c r="D85" s="11">
         <v>44.207560000000001</v>
       </c>
-      <c r="E85" s="24">
+      <c r="E85" s="11">
         <v>109.76472</v>
       </c>
-      <c r="F85" s="24">
+      <c r="F85" s="11">
         <v>153.97228000000001</v>
       </c>
     </row>
     <row r="86" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="22" t="s">
+      <c r="B86" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C86" s="29">
+      <c r="C86" s="16">
         <v>2017</v>
       </c>
-      <c r="D86" s="24">
+      <c r="D86" s="11">
         <v>12.36978</v>
       </c>
-      <c r="E86" s="24">
+      <c r="E86" s="11">
         <v>21.755119999999998</v>
       </c>
-      <c r="F86" s="24">
+      <c r="F86" s="11">
         <v>34.124910000000007</v>
       </c>
     </row>
-    <row r="87" spans="2:6" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="25" t="s">
+    <row r="87" spans="2:6" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C87" s="30">
+      <c r="C87" s="17">
         <v>2017</v>
       </c>
-      <c r="D87" s="27">
+      <c r="D87" s="14">
         <v>452.36584999999997</v>
       </c>
-      <c r="E87" s="27">
+      <c r="E87" s="14">
         <v>333.75468999999998</v>
       </c>
-      <c r="F87" s="27">
+      <c r="F87" s="14">
         <v>786.12054000000001</v>
       </c>
     </row>
     <row r="88" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="22" t="s">
+      <c r="B88" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C88" s="29">
+      <c r="C88" s="16">
         <v>2016</v>
       </c>
-      <c r="D88" s="24">
+      <c r="D88" s="11">
         <v>8.3982800000000015</v>
       </c>
-      <c r="E88" s="24">
+      <c r="E88" s="11">
         <v>3.02813</v>
       </c>
-      <c r="F88" s="24">
+      <c r="F88" s="11">
         <v>11.426410000000001</v>
       </c>
     </row>
     <row r="89" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="22" t="s">
+      <c r="B89" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C89" s="29">
+      <c r="C89" s="16">
         <v>2016</v>
       </c>
-      <c r="D89" s="24">
+      <c r="D89" s="11">
         <v>123.89064</v>
       </c>
-      <c r="E89" s="24">
+      <c r="E89" s="11">
         <v>38.162910000000004</v>
       </c>
-      <c r="F89" s="24">
+      <c r="F89" s="11">
         <v>162.05356</v>
       </c>
     </row>
     <row r="90" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="22" t="s">
+      <c r="B90" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C90" s="29">
+      <c r="C90" s="16">
         <v>2016</v>
       </c>
-      <c r="D90" s="24">
+      <c r="D90" s="11">
         <v>5.1742900000000001</v>
       </c>
-      <c r="E90" s="24">
+      <c r="E90" s="11">
         <v>1.2434700000000001</v>
       </c>
-      <c r="F90" s="24">
+      <c r="F90" s="11">
         <v>6.4177600000000004</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="22" t="s">
+      <c r="B91" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C91" s="29">
+      <c r="C91" s="16">
         <v>2016</v>
       </c>
-      <c r="D91" s="24">
+      <c r="D91" s="11">
         <v>47.020180000000003</v>
       </c>
-      <c r="E91" s="24">
+      <c r="E91" s="11">
         <v>5.593</v>
       </c>
-      <c r="F91" s="24">
+      <c r="F91" s="11">
         <v>52.61318</v>
       </c>
     </row>
     <row r="92" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="22" t="s">
+      <c r="B92" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C92" s="29">
+      <c r="C92" s="16">
         <v>2016</v>
       </c>
-      <c r="D92" s="24">
+      <c r="D92" s="11">
         <v>59.010309999999997</v>
       </c>
-      <c r="E92" s="24">
+      <c r="E92" s="11">
         <v>47.769349999999996</v>
       </c>
-      <c r="F92" s="24">
+      <c r="F92" s="11">
         <v>106.77966000000001</v>
       </c>
     </row>
     <row r="93" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="22" t="s">
+      <c r="B93" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C93" s="29">
+      <c r="C93" s="16">
         <v>2016</v>
       </c>
-      <c r="D93" s="24">
+      <c r="D93" s="11">
         <v>39.857480000000002</v>
       </c>
-      <c r="E93" s="24">
+      <c r="E93" s="11">
         <v>10.64142</v>
       </c>
-      <c r="F93" s="24">
+      <c r="F93" s="11">
         <v>50.498899999999999</v>
       </c>
     </row>
     <row r="94" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="22" t="s">
+      <c r="B94" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C94" s="29">
+      <c r="C94" s="16">
         <v>2016</v>
       </c>
-      <c r="D94" s="24">
+      <c r="D94" s="11">
         <v>25.975009999999997</v>
       </c>
-      <c r="E94" s="24">
+      <c r="E94" s="11">
         <v>22.56588</v>
       </c>
-      <c r="F94" s="24">
+      <c r="F94" s="11">
         <v>48.540900000000001</v>
       </c>
     </row>
     <row r="95" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="22" t="s">
+      <c r="B95" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C95" s="29">
+      <c r="C95" s="16">
         <v>2016</v>
       </c>
-      <c r="D95" s="24">
+      <c r="D95" s="11">
         <v>34.714449999999999</v>
       </c>
-      <c r="E95" s="24">
+      <c r="E95" s="11">
         <v>41.257449999999999</v>
       </c>
-      <c r="F95" s="24">
+      <c r="F95" s="11">
         <v>75.971899999999991</v>
       </c>
     </row>
     <row r="96" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="22" t="s">
+      <c r="B96" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C96" s="29">
+      <c r="C96" s="16">
         <v>2016</v>
       </c>
-      <c r="D96" s="24">
+      <c r="D96" s="11">
         <v>35.625929999999997</v>
       </c>
-      <c r="E96" s="24">
+      <c r="E96" s="11">
         <v>92.135419999999996</v>
       </c>
-      <c r="F96" s="24">
+      <c r="F96" s="11">
         <v>127.76136</v>
       </c>
     </row>
     <row r="97" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="22" t="s">
+      <c r="B97" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C97" s="29">
+      <c r="C97" s="16">
         <v>2016</v>
       </c>
-      <c r="D97" s="24">
+      <c r="D97" s="11">
         <v>9.7516599999999993</v>
       </c>
-      <c r="E97" s="24">
+      <c r="E97" s="11">
         <v>17.925939999999997</v>
       </c>
-      <c r="F97" s="24">
+      <c r="F97" s="11">
         <v>27.677610000000001</v>
       </c>
     </row>
-    <row r="98" spans="2:6" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="25" t="s">
+    <row r="98" spans="2:6" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C98" s="30">
+      <c r="C98" s="17">
         <v>2016</v>
       </c>
-      <c r="D98" s="27">
+      <c r="D98" s="14">
         <v>389.66021000000001</v>
       </c>
-      <c r="E98" s="27">
+      <c r="E98" s="14">
         <v>287.50334999999995</v>
       </c>
-      <c r="F98" s="27">
+      <c r="F98" s="14">
         <v>677.16356999999994</v>
       </c>
     </row>
     <row r="99" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="22" t="s">
+      <c r="B99" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C99" s="23">
+      <c r="C99" s="10">
         <v>2015</v>
       </c>
-      <c r="D99" s="24">
+      <c r="D99" s="11">
         <v>7.4572099999999999</v>
       </c>
-      <c r="E99" s="24">
+      <c r="E99" s="11">
         <v>2.5444599999999999</v>
       </c>
-      <c r="F99" s="24">
+      <c r="F99" s="11">
         <v>10.001670000000001</v>
       </c>
     </row>
     <row r="100" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="22" t="s">
+      <c r="B100" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C100" s="23">
+      <c r="C100" s="10">
         <v>2015</v>
       </c>
-      <c r="D100" s="24">
+      <c r="D100" s="11">
         <v>106.61516</v>
       </c>
-      <c r="E100" s="24">
+      <c r="E100" s="11">
         <v>34.868780000000001</v>
       </c>
-      <c r="F100" s="24">
+      <c r="F100" s="11">
         <v>141.48392999999999</v>
       </c>
     </row>
     <row r="101" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="22" t="s">
+      <c r="B101" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C101" s="23">
+      <c r="C101" s="10">
         <v>2015</v>
       </c>
-      <c r="D101" s="24">
+      <c r="D101" s="11">
         <v>5.0394300000000003</v>
       </c>
-      <c r="E101" s="24">
+      <c r="E101" s="11">
         <v>1.7591600000000001</v>
       </c>
-      <c r="F101" s="24">
+      <c r="F101" s="11">
         <v>6.7985899999999999</v>
       </c>
     </row>
     <row r="102" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="22" t="s">
+      <c r="B102" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C102" s="23">
+      <c r="C102" s="10">
         <v>2015</v>
       </c>
-      <c r="D102" s="24">
+      <c r="D102" s="11">
         <v>42.176349999999999</v>
       </c>
-      <c r="E102" s="24">
+      <c r="E102" s="11">
         <v>3.2217899999999999</v>
       </c>
-      <c r="F102" s="24">
+      <c r="F102" s="11">
         <v>45.398129999999995</v>
       </c>
     </row>
     <row r="103" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="22" t="s">
+      <c r="B103" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C103" s="23">
+      <c r="C103" s="10">
         <v>2015</v>
       </c>
-      <c r="D103" s="24">
+      <c r="D103" s="11">
         <v>57.305949999999996</v>
       </c>
-      <c r="E103" s="24">
+      <c r="E103" s="11">
         <v>43.623470000000005</v>
       </c>
-      <c r="F103" s="24">
+      <c r="F103" s="11">
         <v>100.92941999999999</v>
       </c>
     </row>
     <row r="104" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="22" t="s">
+      <c r="B104" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C104" s="23">
+      <c r="C104" s="10">
         <v>2015</v>
       </c>
-      <c r="D104" s="24">
+      <c r="D104" s="11">
         <v>35.54383</v>
       </c>
-      <c r="E104" s="24">
+      <c r="E104" s="11">
         <v>9.3016699999999997</v>
       </c>
-      <c r="F104" s="24">
+      <c r="F104" s="11">
         <v>44.845500000000001</v>
       </c>
     </row>
     <row r="105" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="22" t="s">
+      <c r="B105" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C105" s="23">
+      <c r="C105" s="10">
         <v>2015</v>
       </c>
-      <c r="D105" s="24">
+      <c r="D105" s="11">
         <v>24.285130000000002</v>
       </c>
-      <c r="E105" s="24">
+      <c r="E105" s="11">
         <v>23.738779999999998</v>
       </c>
-      <c r="F105" s="24">
+      <c r="F105" s="11">
         <v>48.023910000000001</v>
       </c>
     </row>
     <row r="106" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="22" t="s">
+      <c r="B106" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C106" s="23">
+      <c r="C106" s="10">
         <v>2015</v>
       </c>
-      <c r="D106" s="24">
+      <c r="D106" s="11">
         <v>29.162929999999999</v>
       </c>
-      <c r="E106" s="24">
+      <c r="E106" s="11">
         <v>38.966059999999999</v>
       </c>
-      <c r="F106" s="24">
+      <c r="F106" s="11">
         <v>68.128979999999999</v>
       </c>
     </row>
     <row r="107" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="22" t="s">
+      <c r="B107" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C107" s="23">
+      <c r="C107" s="10">
         <v>2015</v>
       </c>
-      <c r="D107" s="24">
+      <c r="D107" s="11">
         <v>29.305509999999998</v>
       </c>
-      <c r="E107" s="24">
+      <c r="E107" s="11">
         <v>88.929559999999995</v>
       </c>
-      <c r="F107" s="24">
+      <c r="F107" s="11">
         <v>118.23508</v>
       </c>
     </row>
     <row r="108" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="22" t="s">
+      <c r="B108" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C108" s="23">
+      <c r="C108" s="10">
         <v>2015</v>
       </c>
-      <c r="D108" s="24">
+      <c r="D108" s="11">
         <v>10.864459999999999</v>
       </c>
-      <c r="E108" s="24">
+      <c r="E108" s="11">
         <v>17.819520000000001</v>
       </c>
-      <c r="F108" s="24">
+      <c r="F108" s="11">
         <v>28.683979999999998</v>
       </c>
     </row>
-    <row r="109" spans="2:6" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="25" t="s">
+    <row r="109" spans="2:6" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C109" s="26">
+      <c r="C109" s="13">
         <v>2015</v>
       </c>
-      <c r="D109" s="27">
+      <c r="D109" s="14">
         <v>348.54129999999998</v>
       </c>
-      <c r="E109" s="27">
+      <c r="E109" s="14">
         <v>268.76832999999999</v>
       </c>
-      <c r="F109" s="27">
+      <c r="F109" s="14">
         <v>617.30962999999997</v>
       </c>
     </row>
     <row r="110" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="22" t="s">
+      <c r="B110" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C110" s="23">
+      <c r="C110" s="10">
         <v>2014</v>
       </c>
-      <c r="D110" s="24">
+      <c r="D110" s="11">
         <v>6.3360699999999994</v>
       </c>
-      <c r="E110" s="24">
+      <c r="E110" s="11">
         <v>3.2820200000000002</v>
       </c>
-      <c r="F110" s="24">
+      <c r="F110" s="11">
         <v>9.6180900000000005</v>
       </c>
     </row>
     <row r="111" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="22" t="s">
+      <c r="B111" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C111" s="23">
+      <c r="C111" s="10">
         <v>2014</v>
       </c>
-      <c r="D111" s="24">
+      <c r="D111" s="11">
         <v>101.78074000000001</v>
       </c>
-      <c r="E111" s="24">
+      <c r="E111" s="11">
         <v>32.59796</v>
       </c>
-      <c r="F111" s="24">
+      <c r="F111" s="11">
         <v>134.37870000000001</v>
       </c>
     </row>
     <row r="112" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="22" t="s">
+      <c r="B112" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C112" s="23">
+      <c r="C112" s="10">
         <v>2014</v>
       </c>
-      <c r="D112" s="24">
+      <c r="D112" s="11">
         <v>5.3153800000000002</v>
       </c>
-      <c r="E112" s="24">
+      <c r="E112" s="11">
         <v>1.54582</v>
       </c>
-      <c r="F112" s="24">
+      <c r="F112" s="11">
         <v>6.8612000000000002</v>
       </c>
     </row>
     <row r="113" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="22" t="s">
+      <c r="B113" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C113" s="23">
+      <c r="C113" s="10">
         <v>2014</v>
       </c>
-      <c r="D113" s="24">
+      <c r="D113" s="11">
         <v>43.502069999999996</v>
       </c>
-      <c r="E113" s="24">
+      <c r="E113" s="11">
         <v>3.6625999999999999</v>
       </c>
-      <c r="F113" s="24">
+      <c r="F113" s="11">
         <v>47.164670000000001</v>
       </c>
     </row>
     <row r="114" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="22" t="s">
+      <c r="B114" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C114" s="23">
+      <c r="C114" s="10">
         <v>2014</v>
       </c>
-      <c r="D114" s="24">
+      <c r="D114" s="11">
         <v>54.192610000000002</v>
       </c>
-      <c r="E114" s="24">
+      <c r="E114" s="11">
         <v>44.216760000000001</v>
       </c>
-      <c r="F114" s="24">
+      <c r="F114" s="11">
         <v>98.409369999999996</v>
       </c>
     </row>
     <row r="115" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="22" t="s">
+      <c r="B115" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C115" s="23">
+      <c r="C115" s="10">
         <v>2014</v>
       </c>
-      <c r="D115" s="24">
+      <c r="D115" s="11">
         <v>32.27196</v>
       </c>
-      <c r="E115" s="24">
+      <c r="E115" s="11">
         <v>9.5218600000000002</v>
       </c>
-      <c r="F115" s="24">
+      <c r="F115" s="11">
         <v>41.793819999999997</v>
       </c>
     </row>
     <row r="116" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="22" t="s">
+      <c r="B116" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C116" s="23">
+      <c r="C116" s="10">
         <v>2014</v>
       </c>
-      <c r="D116" s="24">
+      <c r="D116" s="11">
         <v>22.154979999999998</v>
       </c>
-      <c r="E116" s="24">
+      <c r="E116" s="11">
         <v>21.421209999999999</v>
       </c>
-      <c r="F116" s="24">
+      <c r="F116" s="11">
         <v>43.576180000000001</v>
       </c>
     </row>
     <row r="117" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="22" t="s">
+      <c r="B117" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C117" s="23">
+      <c r="C117" s="10">
         <v>2014</v>
       </c>
-      <c r="D117" s="24">
+      <c r="D117" s="11">
         <v>29.384830000000001</v>
       </c>
-      <c r="E117" s="24">
+      <c r="E117" s="11">
         <v>38.125860000000003</v>
       </c>
-      <c r="F117" s="24">
+      <c r="F117" s="11">
         <v>67.510689999999997</v>
       </c>
     </row>
     <row r="118" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="22" t="s">
+      <c r="B118" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C118" s="23">
+      <c r="C118" s="10">
         <v>2014</v>
       </c>
-      <c r="D118" s="24">
+      <c r="D118" s="11">
         <v>29.18779</v>
       </c>
-      <c r="E118" s="24">
+      <c r="E118" s="11">
         <v>86.626580000000004</v>
       </c>
-      <c r="F118" s="24">
+      <c r="F118" s="11">
         <v>115.81437</v>
       </c>
     </row>
     <row r="119" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="22" t="s">
+      <c r="B119" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C119" s="23">
+      <c r="C119" s="10">
         <v>2014</v>
       </c>
-      <c r="D119" s="24">
+      <c r="D119" s="11">
         <v>10.499379999999999</v>
       </c>
-      <c r="E119" s="24">
+      <c r="E119" s="11">
         <v>18.08278</v>
       </c>
-      <c r="F119" s="24">
+      <c r="F119" s="11">
         <v>28.582159999999998</v>
       </c>
     </row>
-    <row r="120" spans="2:6" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="25" t="s">
+    <row r="120" spans="2:6" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B120" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C120" s="26">
+      <c r="C120" s="13">
         <v>2014</v>
       </c>
-      <c r="D120" s="27">
+      <c r="D120" s="14">
         <v>335.48230000000001</v>
       </c>
-      <c r="E120" s="27">
+      <c r="E120" s="14">
         <v>263.93470000000002</v>
       </c>
-      <c r="F120" s="27">
+      <c r="F120" s="14">
         <v>599.41700000000003</v>
       </c>
     </row>
     <row r="121" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="22" t="s">
+      <c r="B121" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C121" s="23">
+      <c r="C121" s="10">
         <v>2013</v>
       </c>
-      <c r="D121" s="24">
+      <c r="D121" s="11">
         <v>5.6397899999999996</v>
       </c>
-      <c r="E121" s="24">
+      <c r="E121" s="11">
         <v>2.4824999999999999</v>
       </c>
-      <c r="F121" s="24">
+      <c r="F121" s="11">
         <v>8.1222899999999996</v>
       </c>
     </row>
     <row r="122" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="22" t="s">
+      <c r="B122" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C122" s="23">
+      <c r="C122" s="10">
         <v>2013</v>
       </c>
-      <c r="D122" s="24">
+      <c r="D122" s="11">
         <v>97.881570000000011</v>
       </c>
-      <c r="E122" s="24">
+      <c r="E122" s="11">
         <v>31.459490000000002</v>
       </c>
-      <c r="F122" s="24">
+      <c r="F122" s="11">
         <v>129.34106</v>
       </c>
     </row>
     <row r="123" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="22" t="s">
+      <c r="B123" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C123" s="23">
+      <c r="C123" s="10">
         <v>2013</v>
       </c>
-      <c r="D123" s="24">
+      <c r="D123" s="11">
         <v>5.0328999999999997</v>
       </c>
-      <c r="E123" s="24">
+      <c r="E123" s="11">
         <v>2.4439799999999998</v>
       </c>
-      <c r="F123" s="24">
+      <c r="F123" s="11">
         <v>7.4768699999999999</v>
       </c>
     </row>
     <row r="124" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B124" s="22" t="s">
+      <c r="B124" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C124" s="23">
+      <c r="C124" s="10">
         <v>2013</v>
       </c>
-      <c r="D124" s="24">
+      <c r="D124" s="11">
         <v>40.353499999999997</v>
       </c>
-      <c r="E124" s="24">
+      <c r="E124" s="11">
         <v>4.0673899999999996</v>
       </c>
-      <c r="F124" s="24">
+      <c r="F124" s="11">
         <v>44.42089</v>
       </c>
     </row>
     <row r="125" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B125" s="22" t="s">
+      <c r="B125" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C125" s="23">
+      <c r="C125" s="10">
         <v>2013</v>
       </c>
-      <c r="D125" s="24">
+      <c r="D125" s="11">
         <v>56.337489999999995</v>
       </c>
-      <c r="E125" s="24">
+      <c r="E125" s="11">
         <v>45.749169999999999</v>
       </c>
-      <c r="F125" s="24">
+      <c r="F125" s="11">
         <v>102.08666000000001</v>
       </c>
     </row>
     <row r="126" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B126" s="22" t="s">
+      <c r="B126" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C126" s="23">
+      <c r="C126" s="10">
         <v>2013</v>
       </c>
-      <c r="D126" s="24">
+      <c r="D126" s="11">
         <v>32.462830000000004</v>
       </c>
-      <c r="E126" s="24">
+      <c r="E126" s="11">
         <v>9.9921600000000002</v>
       </c>
-      <c r="F126" s="24">
+      <c r="F126" s="11">
         <v>42.454999999999998</v>
       </c>
     </row>
     <row r="127" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="22" t="s">
+      <c r="B127" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C127" s="23">
+      <c r="C127" s="10">
         <v>2013</v>
       </c>
-      <c r="D127" s="24">
+      <c r="D127" s="11">
         <v>24.680419999999998</v>
       </c>
-      <c r="E127" s="24">
+      <c r="E127" s="11">
         <v>23.158660000000001</v>
       </c>
-      <c r="F127" s="24">
+      <c r="F127" s="11">
         <v>47.839080000000003</v>
       </c>
     </row>
     <row r="128" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="22" t="s">
+      <c r="B128" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C128" s="23">
+      <c r="C128" s="10">
         <v>2013</v>
       </c>
-      <c r="D128" s="24">
+      <c r="D128" s="11">
         <v>30.276400000000002</v>
       </c>
-      <c r="E128" s="24">
+      <c r="E128" s="11">
         <v>40.841269999999994</v>
       </c>
-      <c r="F128" s="24">
+      <c r="F128" s="11">
         <v>71.117670000000004</v>
       </c>
     </row>
     <row r="129" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="22" t="s">
+      <c r="B129" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C129" s="23">
+      <c r="C129" s="10">
         <v>2013</v>
       </c>
-      <c r="D129" s="24">
+      <c r="D129" s="11">
         <v>28.304020000000001</v>
       </c>
-      <c r="E129" s="24">
+      <c r="E129" s="11">
         <v>83.318579999999997</v>
       </c>
-      <c r="F129" s="24">
+      <c r="F129" s="11">
         <v>111.62260999999999</v>
       </c>
     </row>
     <row r="130" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="22" t="s">
+      <c r="B130" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C130" s="23">
+      <c r="C130" s="10">
         <v>2013</v>
       </c>
-      <c r="D130" s="24">
+      <c r="D130" s="11">
         <v>10.529069999999999</v>
       </c>
-      <c r="E130" s="24">
+      <c r="E130" s="11">
         <v>19.79946</v>
       </c>
-      <c r="F130" s="24">
+      <c r="F130" s="11">
         <v>30.32854</v>
       </c>
     </row>
-    <row r="131" spans="2:6" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="25" t="s">
+    <row r="131" spans="2:6" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B131" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C131" s="26">
+      <c r="C131" s="13">
         <v>2013</v>
       </c>
-      <c r="D131" s="27">
+      <c r="D131" s="14">
         <v>331.93194</v>
       </c>
-      <c r="E131" s="27">
+      <c r="E131" s="14">
         <v>269.04737</v>
       </c>
-      <c r="F131" s="27">
+      <c r="F131" s="14">
         <v>600.97931000000005</v>
       </c>
     </row>
     <row r="132" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="22" t="s">
+      <c r="B132" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C132" s="23">
+      <c r="C132" s="10">
         <v>2012</v>
       </c>
-      <c r="D132" s="24">
+      <c r="D132" s="11">
         <v>4.7484500000000001</v>
       </c>
-      <c r="E132" s="24">
+      <c r="E132" s="11">
         <v>2.3544999999999998</v>
       </c>
-      <c r="F132" s="24">
+      <c r="F132" s="11">
         <v>7.1029499999999999</v>
       </c>
     </row>
     <row r="133" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B133" s="22" t="s">
+      <c r="B133" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C133" s="23">
+      <c r="C133" s="10">
         <v>2012</v>
       </c>
-      <c r="D133" s="24">
+      <c r="D133" s="11">
         <v>103.27019</v>
       </c>
-      <c r="E133" s="24">
+      <c r="E133" s="11">
         <v>28.397169999999999</v>
       </c>
-      <c r="F133" s="24">
+      <c r="F133" s="11">
         <v>131.66735999999997</v>
       </c>
     </row>
     <row r="134" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="22" t="s">
+      <c r="B134" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C134" s="23">
+      <c r="C134" s="10">
         <v>2012</v>
       </c>
-      <c r="D134" s="24">
+      <c r="D134" s="11">
         <v>4.6591000000000005</v>
       </c>
-      <c r="E134" s="24">
+      <c r="E134" s="11">
         <v>2.0485500000000001</v>
       </c>
-      <c r="F134" s="24">
+      <c r="F134" s="11">
         <v>6.7076599999999997</v>
       </c>
     </row>
     <row r="135" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="22" t="s">
+      <c r="B135" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C135" s="23">
+      <c r="C135" s="10">
         <v>2012</v>
       </c>
-      <c r="D135" s="24">
+      <c r="D135" s="11">
         <v>36.897529999999996</v>
       </c>
-      <c r="E135" s="24">
+      <c r="E135" s="11">
         <v>3.5321599999999997</v>
       </c>
-      <c r="F135" s="24">
+      <c r="F135" s="11">
         <v>40.429690000000001</v>
       </c>
     </row>
     <row r="136" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="22" t="s">
+      <c r="B136" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C136" s="23">
+      <c r="C136" s="10">
         <v>2012</v>
       </c>
-      <c r="D136" s="24">
+      <c r="D136" s="11">
         <v>42.788410000000006</v>
       </c>
-      <c r="E136" s="24">
+      <c r="E136" s="11">
         <v>40.614100000000001</v>
       </c>
-      <c r="F136" s="24">
+      <c r="F136" s="11">
         <v>83.402509999999992</v>
       </c>
     </row>
     <row r="137" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="22" t="s">
+      <c r="B137" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C137" s="23">
+      <c r="C137" s="10">
         <v>2012</v>
       </c>
-      <c r="D137" s="24">
+      <c r="D137" s="11">
         <v>30.841380000000001</v>
       </c>
-      <c r="E137" s="24">
+      <c r="E137" s="11">
         <v>8.6682299999999994</v>
       </c>
-      <c r="F137" s="24">
+      <c r="F137" s="11">
         <v>39.509610000000002</v>
       </c>
     </row>
     <row r="138" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="22" t="s">
+      <c r="B138" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C138" s="23">
+      <c r="C138" s="10">
         <v>2012</v>
       </c>
-      <c r="D138" s="24">
+      <c r="D138" s="11">
         <v>21.644099999999998</v>
       </c>
-      <c r="E138" s="24">
+      <c r="E138" s="11">
         <v>23.704169999999998</v>
       </c>
-      <c r="F138" s="24">
+      <c r="F138" s="11">
         <v>45.348269999999999</v>
       </c>
     </row>
     <row r="139" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B139" s="22" t="s">
+      <c r="B139" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C139" s="23">
+      <c r="C139" s="10">
         <v>2012</v>
       </c>
-      <c r="D139" s="24">
+      <c r="D139" s="11">
         <v>30.431819999999998</v>
       </c>
-      <c r="E139" s="24">
+      <c r="E139" s="11">
         <v>34.406230000000001</v>
       </c>
-      <c r="F139" s="24">
+      <c r="F139" s="11">
         <v>64.83805000000001</v>
       </c>
     </row>
     <row r="140" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B140" s="22" t="s">
+      <c r="B140" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C140" s="23">
+      <c r="C140" s="10">
         <v>2012</v>
       </c>
-      <c r="D140" s="24">
+      <c r="D140" s="11">
         <v>27.84985</v>
       </c>
-      <c r="E140" s="24">
+      <c r="E140" s="11">
         <v>79.877619999999993</v>
       </c>
-      <c r="F140" s="24">
+      <c r="F140" s="11">
         <v>107.72747</v>
       </c>
     </row>
     <row r="141" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="22" t="s">
+      <c r="B141" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C141" s="23">
+      <c r="C141" s="10">
         <v>2012</v>
       </c>
-      <c r="D141" s="24">
+      <c r="D141" s="11">
         <v>10.02529</v>
       </c>
-      <c r="E141" s="24">
+      <c r="E141" s="11">
         <v>21.0427</v>
       </c>
-      <c r="F141" s="24">
+      <c r="F141" s="11">
         <v>31.068000000000001</v>
       </c>
     </row>
-    <row r="142" spans="2:6" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="25" t="s">
+    <row r="142" spans="2:6" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B142" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C142" s="26">
+      <c r="C142" s="13">
         <v>2012</v>
       </c>
-      <c r="D142" s="27">
+      <c r="D142" s="14">
         <v>314.28734000000003</v>
       </c>
-      <c r="E142" s="27">
+      <c r="E142" s="14">
         <v>251.34277</v>
       </c>
-      <c r="F142" s="27">
+      <c r="F142" s="14">
         <v>565.63010999999995</v>
       </c>
     </row>
-    <row r="143" spans="2:6" s="31" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="22" t="s">
+    <row r="143" spans="2:6" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B143" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C143" s="23">
+      <c r="C143" s="10">
         <v>2011</v>
       </c>
-      <c r="D143" s="24">
+      <c r="D143" s="11">
         <v>6.9908100000000006</v>
       </c>
-      <c r="E143" s="24">
+      <c r="E143" s="11">
         <v>2.84619</v>
       </c>
-      <c r="F143" s="24">
+      <c r="F143" s="11">
         <v>9.8370099999999994</v>
       </c>
     </row>
-    <row r="144" spans="2:6" s="31" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B144" s="22" t="s">
+    <row r="144" spans="2:6" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B144" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C144" s="23">
+      <c r="C144" s="10">
         <v>2011</v>
       </c>
-      <c r="D144" s="24">
+      <c r="D144" s="11">
         <v>97.082039999999992</v>
       </c>
-      <c r="E144" s="24">
+      <c r="E144" s="11">
         <v>30.17259</v>
       </c>
-      <c r="F144" s="24">
+      <c r="F144" s="11">
         <v>127.25463000000001</v>
       </c>
     </row>
-    <row r="145" spans="2:6" s="31" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="22" t="s">
+    <row r="145" spans="2:6" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B145" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C145" s="23">
+      <c r="C145" s="10">
         <v>2011</v>
       </c>
-      <c r="D145" s="24">
+      <c r="D145" s="11">
         <v>6.2511599999999996</v>
       </c>
-      <c r="E145" s="24">
+      <c r="E145" s="11">
         <v>1.1867399999999999</v>
       </c>
-      <c r="F145" s="24">
+      <c r="F145" s="11">
         <v>7.4378900000000003</v>
       </c>
     </row>
-    <row r="146" spans="2:6" s="31" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B146" s="22" t="s">
+    <row r="146" spans="2:6" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B146" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C146" s="23">
+      <c r="C146" s="10">
         <v>2011</v>
       </c>
-      <c r="D146" s="24">
+      <c r="D146" s="11">
         <v>37.432389999999998</v>
       </c>
-      <c r="E146" s="24">
+      <c r="E146" s="11">
         <v>3.95919</v>
       </c>
-      <c r="F146" s="24">
+      <c r="F146" s="11">
         <v>41.391580000000005</v>
       </c>
     </row>
-    <row r="147" spans="2:6" s="31" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B147" s="22" t="s">
+    <row r="147" spans="2:6" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B147" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C147" s="23">
+      <c r="C147" s="10">
         <v>2011</v>
       </c>
-      <c r="D147" s="24">
+      <c r="D147" s="11">
         <v>44.099319999999999</v>
       </c>
-      <c r="E147" s="24">
+      <c r="E147" s="11">
         <v>42.393800000000006</v>
       </c>
-      <c r="F147" s="24">
+      <c r="F147" s="11">
         <v>86.493110000000001</v>
       </c>
     </row>
-    <row r="148" spans="2:6" s="31" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B148" s="22" t="s">
+    <row r="148" spans="2:6" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B148" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C148" s="23">
+      <c r="C148" s="10">
         <v>2011</v>
       </c>
-      <c r="D148" s="24">
+      <c r="D148" s="11">
         <v>28.452869999999997</v>
       </c>
-      <c r="E148" s="24">
+      <c r="E148" s="11">
         <v>7.19041</v>
       </c>
-      <c r="F148" s="24">
+      <c r="F148" s="11">
         <v>35.643279999999997</v>
       </c>
     </row>
-    <row r="149" spans="2:6" s="31" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="22" t="s">
+    <row r="149" spans="2:6" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B149" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C149" s="23">
+      <c r="C149" s="10">
         <v>2011</v>
       </c>
-      <c r="D149" s="24">
+      <c r="D149" s="11">
         <v>21.702169999999999</v>
       </c>
-      <c r="E149" s="24">
+      <c r="E149" s="11">
         <v>21.758330000000001</v>
       </c>
-      <c r="F149" s="24">
+      <c r="F149" s="11">
         <v>43.460500000000003</v>
       </c>
     </row>
-    <row r="150" spans="2:6" s="31" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B150" s="22" t="s">
+    <row r="150" spans="2:6" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B150" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C150" s="23">
+      <c r="C150" s="10">
         <v>2011</v>
       </c>
-      <c r="D150" s="24">
+      <c r="D150" s="11">
         <v>28.261490000000002</v>
       </c>
-      <c r="E150" s="24">
+      <c r="E150" s="11">
         <v>37.508559999999996</v>
       </c>
-      <c r="F150" s="24">
+      <c r="F150" s="11">
         <v>65.770049999999998</v>
       </c>
     </row>
-    <row r="151" spans="2:6" s="31" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="22" t="s">
+    <row r="151" spans="2:6" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B151" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C151" s="23">
+      <c r="C151" s="10">
         <v>2011</v>
       </c>
-      <c r="D151" s="24">
+      <c r="D151" s="11">
         <v>25.228020000000001</v>
       </c>
-      <c r="E151" s="24">
+      <c r="E151" s="11">
         <v>76.428370000000001</v>
       </c>
-      <c r="F151" s="24">
+      <c r="F151" s="11">
         <v>101.65639</v>
       </c>
     </row>
-    <row r="152" spans="2:6" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B152" s="22" t="s">
+    <row r="152" spans="2:6" s="18" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C152" s="23">
+      <c r="C152" s="10">
         <v>2011</v>
       </c>
-      <c r="D152" s="24">
+      <c r="D152" s="11">
         <v>7.7126000000000001</v>
       </c>
-      <c r="E152" s="24">
+      <c r="E152" s="11">
         <v>16.179190000000002</v>
       </c>
-      <c r="F152" s="24">
+      <c r="F152" s="11">
         <v>23.8918</v>
       </c>
     </row>
-    <row r="153" spans="2:6" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B153" s="25" t="s">
+    <row r="153" spans="2:6" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B153" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C153" s="26">
+      <c r="C153" s="13">
         <v>2011</v>
       </c>
-      <c r="D153" s="27">
+      <c r="D153" s="14">
         <v>303.62559000000005</v>
       </c>
-      <c r="E153" s="27">
+      <c r="E153" s="14">
         <v>245.06873999999999</v>
       </c>
-      <c r="F153" s="27">
+      <c r="F153" s="14">
         <v>548.69432999999992</v>
       </c>
     </row>
     <row r="154" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B154" s="22" t="s">
+      <c r="B154" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C154" s="23">
+      <c r="C154" s="10">
         <v>2010</v>
       </c>
-      <c r="D154" s="24">
+      <c r="D154" s="11">
         <v>5.15707</v>
       </c>
-      <c r="E154" s="32" t="s">
+      <c r="E154" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F154" s="24">
+      <c r="F154" s="11">
         <v>7.90266</v>
       </c>
     </row>
     <row r="155" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B155" s="22" t="s">
+      <c r="B155" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C155" s="23">
+      <c r="C155" s="10">
         <v>2010</v>
       </c>
-      <c r="D155" s="24">
+      <c r="D155" s="11">
         <v>99.316779999999994</v>
       </c>
-      <c r="E155" s="24">
+      <c r="E155" s="11">
         <v>30.532409999999999</v>
       </c>
-      <c r="F155" s="24">
+      <c r="F155" s="11">
         <v>129.84918999999999</v>
       </c>
     </row>
     <row r="156" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B156" s="22" t="s">
+      <c r="B156" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C156" s="23">
+      <c r="C156" s="10">
         <v>2010</v>
       </c>
-      <c r="D156" s="32" t="s">
+      <c r="D156" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="E156" s="32" t="s">
+      <c r="E156" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F156" s="24">
+      <c r="F156" s="11">
         <v>6.0895600000000005</v>
       </c>
     </row>
     <row r="157" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B157" s="22" t="s">
+      <c r="B157" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C157" s="23">
+      <c r="C157" s="10">
         <v>2010</v>
       </c>
-      <c r="D157" s="24">
+      <c r="D157" s="11">
         <v>34.972910000000006</v>
       </c>
-      <c r="E157" s="32" t="s">
+      <c r="E157" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F157" s="24">
+      <c r="F157" s="11">
         <v>38.963010000000004</v>
       </c>
     </row>
     <row r="158" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B158" s="22" t="s">
+      <c r="B158" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C158" s="23">
+      <c r="C158" s="10">
         <v>2010</v>
       </c>
-      <c r="D158" s="24">
+      <c r="D158" s="11">
         <v>44.276260000000001</v>
       </c>
-      <c r="E158" s="24">
+      <c r="E158" s="11">
         <v>38.775419999999997</v>
       </c>
-      <c r="F158" s="24">
+      <c r="F158" s="11">
         <v>83.05167999999999</v>
       </c>
     </row>
     <row r="159" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="22" t="s">
+      <c r="B159" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C159" s="23">
+      <c r="C159" s="10">
         <v>2010</v>
       </c>
-      <c r="D159" s="24">
+      <c r="D159" s="11">
         <v>28.7331</v>
       </c>
-      <c r="E159" s="24">
+      <c r="E159" s="11">
         <v>7.50441</v>
       </c>
-      <c r="F159" s="24">
+      <c r="F159" s="11">
         <v>36.23751</v>
       </c>
     </row>
     <row r="160" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="22" t="s">
+      <c r="B160" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C160" s="23">
+      <c r="C160" s="10">
         <v>2010</v>
       </c>
-      <c r="D160" s="24">
+      <c r="D160" s="11">
         <v>22.546250000000001</v>
       </c>
-      <c r="E160" s="24">
+      <c r="E160" s="11">
         <v>20.54298</v>
       </c>
-      <c r="F160" s="24">
+      <c r="F160" s="11">
         <v>43.089230000000001</v>
       </c>
     </row>
     <row r="161" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B161" s="22" t="s">
+      <c r="B161" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C161" s="23">
+      <c r="C161" s="10">
         <v>2010</v>
       </c>
-      <c r="D161" s="24">
+      <c r="D161" s="11">
         <v>30.43019</v>
       </c>
-      <c r="E161" s="24">
+      <c r="E161" s="11">
         <v>35.658290000000001</v>
       </c>
-      <c r="F161" s="24">
+      <c r="F161" s="11">
         <v>66.08847999999999</v>
       </c>
     </row>
     <row r="162" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B162" s="22" t="s">
+      <c r="B162" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C162" s="23">
+      <c r="C162" s="10">
         <v>2010</v>
       </c>
-      <c r="D162" s="24">
+      <c r="D162" s="11">
         <v>30.262689999999999</v>
       </c>
-      <c r="E162" s="24">
+      <c r="E162" s="11">
         <v>79.982199999999992</v>
       </c>
-      <c r="F162" s="24">
+      <c r="F162" s="11">
         <v>110.24489</v>
       </c>
     </row>
     <row r="163" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B163" s="22" t="s">
+      <c r="B163" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C163" s="23">
+      <c r="C163" s="10">
         <v>2010</v>
       </c>
-      <c r="D163" s="24">
+      <c r="D163" s="11">
         <v>8.6783999999999999</v>
       </c>
-      <c r="E163" s="24">
+      <c r="E163" s="11">
         <v>17.198979999999999</v>
       </c>
-      <c r="F163" s="24">
+      <c r="F163" s="11">
         <v>25.877380000000002</v>
       </c>
     </row>
-    <row r="164" spans="2:9" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B164" s="25" t="s">
+    <row r="164" spans="2:9" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B164" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C164" s="26">
+      <c r="C164" s="13">
         <v>2010</v>
       </c>
-      <c r="D164" s="27">
+      <c r="D164" s="14">
         <v>309.77222999999998</v>
       </c>
-      <c r="E164" s="27">
+      <c r="E164" s="14">
         <v>243.49507</v>
       </c>
-      <c r="F164" s="27">
+      <c r="F164" s="14">
         <v>553.26731000000007</v>
       </c>
     </row>
     <row r="165" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D165" s="33"/>
-      <c r="E165" s="33"/>
+      <c r="D165" s="20"/>
+      <c r="E165" s="20"/>
     </row>
     <row r="166" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B166" s="34" t="s">
+      <c r="B166" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="C166" s="34"/>
-      <c r="D166" s="34"/>
-      <c r="E166" s="34"/>
-      <c r="F166" s="34"/>
+      <c r="C166" s="47"/>
+      <c r="D166" s="47"/>
+      <c r="E166" s="47"/>
+      <c r="F166" s="47"/>
     </row>
     <row r="167" spans="2:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B167" s="34" t="s">
+      <c r="B167" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C167" s="34"/>
-      <c r="D167" s="34"/>
-      <c r="E167" s="34"/>
-      <c r="F167" s="35"/>
+      <c r="C167" s="47"/>
+      <c r="D167" s="47"/>
+      <c r="E167" s="47"/>
+      <c r="F167" s="48"/>
     </row>
     <row r="168" spans="2:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B168" s="36" t="s">
+      <c r="B168" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C168" s="36"/>
-      <c r="D168" s="36"/>
-      <c r="E168" s="36"/>
-      <c r="F168" s="36"/>
-      <c r="G168" s="37"/>
-      <c r="H168" s="37"/>
-      <c r="I168" s="37"/>
+      <c r="C168" s="32"/>
+      <c r="D168" s="32"/>
+      <c r="E168" s="32"/>
+      <c r="F168" s="32"/>
+      <c r="G168" s="21"/>
+      <c r="H168" s="21"/>
+      <c r="I168" s="21"/>
     </row>
     <row r="169" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B169" s="38" t="s">
+      <c r="B169" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C169" s="38"/>
-      <c r="D169" s="38"/>
-      <c r="E169" s="38"/>
-      <c r="F169" s="38"/>
-      <c r="G169" s="38"/>
-      <c r="H169" s="38"/>
-      <c r="I169" s="38"/>
+      <c r="C169" s="33"/>
+      <c r="D169" s="33"/>
+      <c r="E169" s="33"/>
+      <c r="F169" s="33"/>
+      <c r="G169" s="33"/>
+      <c r="H169" s="33"/>
+      <c r="I169" s="33"/>
     </row>
     <row r="170" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B170" s="39" t="s">
+      <c r="B170" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C170" s="39"/>
+      <c r="C170" s="22"/>
     </row>
     <row r="172" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B172" s="39" t="s">
+      <c r="B172" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C172" s="39"/>
+      <c r="C172" s="22"/>
     </row>
     <row r="173" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B173" s="40" t="s">
+      <c r="B173" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C173" s="39"/>
+      <c r="C173" s="22"/>
     </row>
     <row r="174" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B174" s="39" t="s">
+      <c r="B174" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C174" s="39"/>
+      <c r="C174" s="22"/>
     </row>
     <row r="175" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B175" s="41" t="s">
+      <c r="B175" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C175" s="39"/>
+      <c r="C175" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>